<commit_message>
preenchida a tabela de riscos de projetos
</commit_message>
<xml_diff>
--- a/documentacao/riscos_projeto.xlsx
+++ b/documentacao/riscos_projeto.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABD4EA2-8352-4543-9A24-486EC14A7982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1584E07-3EC3-4E85-9A9B-797ADC1E6080}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16427E0A-EFB0-45BE-B62C-D4DFB6F43843}"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -73,6 +67,36 @@
   </si>
   <si>
     <t>3 - Alta</t>
+  </si>
+  <si>
+    <t>Funcionário faltar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problemas na infraestrutura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perda de informações e dados essenciais </t>
+  </si>
+  <si>
+    <t>Ajuestes não realizados dentro do prazo</t>
+  </si>
+  <si>
+    <t>Reclamações do usuário devido a bugs</t>
+  </si>
+  <si>
+    <t>Nova adequação e redistribuição da equipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer analise preventiva todo dia </t>
+  </si>
+  <si>
+    <t>Ter protocolo de backups após todas atualizações</t>
+  </si>
+  <si>
+    <t>Ter cronograma e planejamento de odo o projeto</t>
+  </si>
+  <si>
+    <t>Garantir que a homologação foi feita de maneira acertiva]</t>
   </si>
 </sst>
 </file>
@@ -131,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,22 +172,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -504,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952895F1-EA09-4CEC-9F68-1AD05237DED7}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +534,7 @@
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="7" max="7" width="45.42578125" customWidth="1"/>
+    <col min="7" max="7" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -542,99 +560,134 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <f>SUM(C2*D2)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E11" si="0">SUM(C3*D3)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
@@ -655,6 +708,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -672,6 +726,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -689,6 +744,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -706,6 +762,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -723,6 +780,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -741,6 +799,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -828,17 +887,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>0</formula>
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
@@ -855,6 +914,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações na planilha de riscos
</commit_message>
<xml_diff>
--- a/documentacao/riscos_projeto.xlsx
+++ b/documentacao/riscos_projeto.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1584E07-3EC3-4E85-9A9B-797ADC1E6080}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF72F79-8A87-4FEA-BEC8-22BFE3345891}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16427E0A-EFB0-45BE-B62C-D4DFB6F43843}"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -72,31 +78,37 @@
     <t>Funcionário faltar</t>
   </si>
   <si>
-    <t xml:space="preserve">problemas na infraestrutura </t>
-  </si>
-  <si>
     <t xml:space="preserve">Perda de informações e dados essenciais </t>
   </si>
   <si>
-    <t>Ajuestes não realizados dentro do prazo</t>
-  </si>
-  <si>
     <t>Reclamações do usuário devido a bugs</t>
   </si>
   <si>
-    <t>Nova adequação e redistribuição da equipe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fazer analise preventiva todo dia </t>
   </si>
   <si>
     <t>Ter protocolo de backups após todas atualizações</t>
   </si>
   <si>
-    <t>Ter cronograma e planejamento de odo o projeto</t>
-  </si>
-  <si>
-    <t>Garantir que a homologação foi feita de maneira acertiva]</t>
+    <t xml:space="preserve">Redistibuir equipe para atender as novas necessidades </t>
+  </si>
+  <si>
+    <t>Problemas na infraestrutura (Falhas nos sensores)</t>
+  </si>
+  <si>
+    <t>Ajustes não realizados dentro do prazo</t>
+  </si>
+  <si>
+    <t>Ter cronograma e planejamento de todo o projeto</t>
+  </si>
+  <si>
+    <t>Garantir que a homologação foi feita de maneira acertiva</t>
+  </si>
+  <si>
+    <t>Não ter Wifi no dia da apresentação</t>
+  </si>
+  <si>
+    <t>Ter todos os arquivos em diferentes pen drivers</t>
   </si>
 </sst>
 </file>
@@ -155,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +185,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,14 +203,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -522,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952895F1-EA09-4CEC-9F68-1AD05237DED7}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +549,7 @@
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="7" max="7" width="53" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -589,7 +604,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -605,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -616,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -632,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -643,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -670,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -696,89 +711,59 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
@@ -788,7 +773,6 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -893,13 +877,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>1</formula>
       <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>3</formula>
-      <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">

</xml_diff>

<commit_message>
Tela Conta do site interno - Raissa A
</commit_message>
<xml_diff>
--- a/documentacao/riscos_projeto.xlsx
+++ b/documentacao/riscos_projeto.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF72F79-8A87-4FEA-BEC8-22BFE3345891}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16427E0A-EFB0-45BE-B62C-D4DFB6F43843}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,9 +74,6 @@
     <t>3 - Alta</t>
   </si>
   <si>
-    <t>Funcionário faltar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Perda de informações e dados essenciais </t>
   </si>
   <si>
@@ -109,12 +105,15 @@
   </si>
   <si>
     <t>Ter todos os arquivos em diferentes pen drivers</t>
+  </si>
+  <si>
+    <t>Integrante da equipe faltar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,11 +533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952895F1-EA09-4CEC-9F68-1AD05237DED7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,8 +578,8 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -596,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -604,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -613,14 +612,14 @@
         <v>3</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E11" si="0">SUM(C3*D3)</f>
+        <f t="shared" ref="E3:E7" si="0">SUM(C3*D3)</f>
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -631,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -647,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -658,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -674,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
@@ -685,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -701,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -712,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -728,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -893,7 +892,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{6D2EE0DA-8CF3-4471-8E67-E5F49314068B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
       <formula1>$I$3:$I$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
atualizada planilha de risco, de acordo com as orientações do Prof"
 git commit -matualizado!
</commit_message>
<xml_diff>
--- a/documentacao/riscos_projeto.xlsx
+++ b/documentacao/riscos_projeto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teodoro\Desktop\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D64D7EF-766D-4D35-AF3D-B0F8624943E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5FF9D4-0AF3-4F14-AEFE-FFA1C6FAEB6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Transferir</t>
   </si>
   <si>
-    <t>Aceitar</t>
-  </si>
-  <si>
     <t>1 - Baixa</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t xml:space="preserve">Perda de informações e dados essenciais </t>
   </si>
   <si>
-    <t>Reclamações do usuário devido a bugs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fazer analise preventiva todo dia </t>
   </si>
   <si>
@@ -97,9 +91,6 @@
   </si>
   <si>
     <t>Ter cronograma e planejamento de todo o projeto</t>
-  </si>
-  <si>
-    <t>Garantir que a homologação foi feita de maneira acertiva</t>
   </si>
   <si>
     <t>Não ter Wifi no dia da apresentação</t>
@@ -538,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -599,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -607,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -616,14 +607,14 @@
         <v>3</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E7" si="0">SUM(C3*D3)</f>
+        <f t="shared" ref="E3:E6" si="0">SUM(C3*D3)</f>
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -634,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -650,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -661,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -677,62 +668,44 @@
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -740,22 +713,22 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="2"/>
       <c r="E10" s="7"/>
       <c r="F10" s="1"/>
@@ -766,16 +739,18 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -786,7 +761,6 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -801,9 +775,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -864,22 +836,14 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E11">
+  <conditionalFormatting sqref="E2:E10">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>0</formula>
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E11">
+  <conditionalFormatting sqref="E2:E10">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>3</formula>
       <formula>4</formula>
@@ -889,15 +853,15 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E11">
+  <conditionalFormatting sqref="E2:E10">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>5</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$I$3:$I$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$I$3:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>